<commit_message>
addressing first reviewer comments
</commit_message>
<xml_diff>
--- a/data/test_run/iTURBO2_input_ash_experiment_test_run.xlsx
+++ b/data/test_run/iTURBO2_input_ash_experiment_test_run.xlsx
@@ -401,8 +401,8 @@
   </sheetPr>
   <dimension ref="A1:Z104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52:F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3591,34 +3591,174 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10"/>
+      <c r="A64" s="10" t="n">
+        <v>61</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10"/>
+      <c r="A65" s="10" t="n">
+        <v>62</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10"/>
+      <c r="A66" s="10" t="n">
+        <v>63</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="10"/>
+      <c r="A67" s="10" t="n">
+        <v>64</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10"/>
+      <c r="A68" s="10" t="n">
+        <v>65</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="10"/>
+      <c r="A69" s="10" t="n">
+        <v>66</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="10"/>
+      <c r="A70" s="10" t="n">
+        <v>67</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="10"/>
+      <c r="A71" s="10" t="n">
+        <v>68</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="10"/>
+      <c r="A72" s="10" t="n">
+        <v>69</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="10"/>
+      <c r="A73" s="10" t="n">
+        <v>70</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="10"/>

</xml_diff>